<commit_message>
Merging units in JRC data
</commit_message>
<xml_diff>
--- a/grouped.xlsx
+++ b/grouped.xlsx
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>928</v>
+        <v>1898</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>928</v>
+        <v>1898</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>928</v>
+        <v>1898</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -774,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>928</v>
+        <v>1898</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1506</v>
+        <v>3304</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>2221</v>
+        <v>3304</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>2871</v>
+        <v>3699</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1177,7 +1177,7 @@
         <v>253</v>
       </c>
       <c r="E3">
-        <v>3385</v>
+        <v>3825</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1070</v>
+        <v>6213</v>
       </c>
       <c r="M3">
         <v>1275</v>
@@ -1221,7 +1221,7 @@
         <v>253</v>
       </c>
       <c r="E4">
-        <v>6198</v>
+        <v>7578</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>2575</v>
+        <v>6793</v>
       </c>
       <c r="M4">
         <v>1275</v>
@@ -1265,13 +1265,13 @@
         <v>253</v>
       </c>
       <c r="E5">
-        <v>6518</v>
+        <v>7578</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>6719</v>
+        <v>9891</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1286,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>6955</v>
+        <v>11005</v>
       </c>
       <c r="M5">
         <v>1275</v>
@@ -1309,13 +1309,13 @@
         <v>253</v>
       </c>
       <c r="E6">
-        <v>9048</v>
+        <v>10108</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>9516</v>
+        <v>12865</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1330,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>8561</v>
+        <v>13475</v>
       </c>
       <c r="M6">
         <v>2677</v>
@@ -1353,13 +1353,13 @@
         <v>253</v>
       </c>
       <c r="E7">
-        <v>16341</v>
+        <v>18758</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>9516</v>
+        <v>12865</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>10913</v>
+        <v>16825</v>
       </c>
       <c r="M7">
         <v>6609</v>
@@ -1397,13 +1397,13 @@
         <v>815.8</v>
       </c>
       <c r="E8">
-        <v>19493</v>
+        <v>22176</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>9941</v>
+        <v>13290</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1418,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>11911</v>
+        <v>16825</v>
       </c>
       <c r="M8">
         <v>12085</v>
@@ -1441,13 +1441,13 @@
         <v>815.8</v>
       </c>
       <c r="E9">
-        <v>20340</v>
+        <v>23023</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>11294</v>
+        <v>14133</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>12361</v>
+        <v>17725</v>
       </c>
       <c r="M9">
         <v>12085</v>
@@ -1485,13 +1485,13 @@
         <v>943.6</v>
       </c>
       <c r="E10">
-        <v>20799</v>
+        <v>23146</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>13601</v>
+        <v>16440</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>16103</v>
+        <v>21017</v>
       </c>
       <c r="M10">
         <v>12085</v>
@@ -1529,13 +1529,13 @@
         <v>1394.9</v>
       </c>
       <c r="E11">
-        <v>20799</v>
+        <v>23146</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>15624</v>
+        <v>17901</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1550,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>17867</v>
+        <v>21017</v>
       </c>
       <c r="M11">
         <v>12085</v>
@@ -1573,7 +1573,7 @@
         <v>1655.3</v>
       </c>
       <c r="E12">
-        <v>21122</v>
+        <v>23469</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1594,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>18267</v>
+        <v>21017</v>
       </c>
       <c r="M12">
         <v>12085</v>
@@ -1661,13 +1661,13 @@
         <v>1655.3</v>
       </c>
       <c r="E14">
-        <v>25051</v>
+        <v>23971</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>21302</v>
+        <v>19168</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1682,10 +1682,10 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>19677</v>
+        <v>16888</v>
       </c>
       <c r="M14">
-        <v>9526</v>
+        <v>8238</v>
       </c>
       <c r="N14">
         <v>1418</v>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>914</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>914</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2573,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>801</v>
+        <v>1258</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2611,13 +2611,13 @@
         <v>137</v>
       </c>
       <c r="E7">
-        <v>285</v>
+        <v>855</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1072</v>
+        <v>1529</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -2661,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1072</v>
+        <v>1529</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1535</v>
+        <v>1992</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1535</v>
+        <v>1992</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -2793,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>2444</v>
+        <v>3245</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -2881,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>4137</v>
+        <v>4029</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>4137</v>
+        <v>4029</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -3026,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>682.9000000000001</v>
+        <v>607.8000000000001</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3041,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>159</v>
+        <v>962</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -3070,7 +3070,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>682.9000000000001</v>
+        <v>607.8000000000001</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -3085,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>379</v>
+        <v>1182</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -3114,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>682.9000000000001</v>
+        <v>607.8000000000001</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3129,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>379</v>
+        <v>1182</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1333.9</v>
+        <v>1448.8</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3173,7 +3173,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>379</v>
+        <v>1182</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -3202,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2329.9</v>
+        <v>2312.8</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3217,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1166</v>
+        <v>1182</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -3246,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>2329.9</v>
+        <v>2312.8</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3264,7 +3264,7 @@
         <v>1182</v>
       </c>
       <c r="M7">
-        <v>955.4</v>
+        <v>1899.4</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -3290,7 +3290,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>2329.9</v>
+        <v>2312.8</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -3655,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>6847</v>
+        <v>6862</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3676,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>2953</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3693,13 +3693,13 @@
         <v>571</v>
       </c>
       <c r="E3">
-        <v>432</v>
+        <v>594</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7235</v>
+        <v>7615</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -3737,13 +3737,13 @@
         <v>571</v>
       </c>
       <c r="E4">
-        <v>1144</v>
+        <v>1886</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>8314</v>
+        <v>8694</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3781,13 +3781,13 @@
         <v>571</v>
       </c>
       <c r="E5">
-        <v>2297</v>
+        <v>2479</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>8622</v>
+        <v>10182</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>3860</v>
+        <v>4148</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3825,13 +3825,13 @@
         <v>571</v>
       </c>
       <c r="E6">
-        <v>2297</v>
+        <v>2479</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>9020</v>
+        <v>10580</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3869,13 +3869,13 @@
         <v>571</v>
       </c>
       <c r="E7">
-        <v>2297</v>
+        <v>2479</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>9420</v>
+        <v>10980</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3919,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>9420</v>
+        <v>10980</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -3963,7 +3963,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>9907</v>
+        <v>11102</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -4007,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>13814</v>
+        <v>15009</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -4051,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>26817</v>
+        <v>27437</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -4160,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>4493</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -4913,7 +4913,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>660</v>
+        <v>2005</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4957,7 +4957,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>660</v>
+        <v>2005</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -5001,7 +5001,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1260</v>
+        <v>2005</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -5045,7 +5045,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1560</v>
+        <v>2005</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -5089,7 +5089,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1670</v>
+        <v>2115</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -5133,7 +5133,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1670</v>
+        <v>2115</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -5177,7 +5177,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1670</v>
+        <v>2115</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -5221,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1670</v>
+        <v>2115</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -5265,7 +5265,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1670</v>
+        <v>2115</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -5309,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1670</v>
+        <v>2115</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -5441,7 +5441,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1515</v>
+        <v>470</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -6794,13 +6794,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1019</v>
+        <v>408</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2029</v>
+        <v>1607</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -6838,13 +6838,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1019</v>
+        <v>408</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>2029</v>
+        <v>1607</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -6882,13 +6882,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1019</v>
+        <v>408</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>2029</v>
+        <v>1607</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -6926,13 +6926,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2089</v>
+        <v>1478</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>2379</v>
+        <v>2476</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -6976,7 +6976,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>3563</v>
+        <v>4964</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -7020,7 +7020,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>3563</v>
+        <v>4964</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -7064,7 +7064,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>3938</v>
+        <v>4964</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -7102,13 +7102,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>3382</v>
+        <v>3822</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>5266</v>
+        <v>6727</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -7146,13 +7146,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>3382</v>
+        <v>3822</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>7362</v>
+        <v>9097</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -7190,13 +7190,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>3382</v>
+        <v>3822</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>8202</v>
+        <v>9937</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -7234,13 +7234,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3382</v>
+        <v>3822</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>11354</v>
+        <v>11785</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -7284,7 +7284,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>12735</v>
+        <v>14039</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -7322,13 +7322,13 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>5114</v>
+        <v>4471</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>11777</v>
+        <v>11359</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -8586,7 +8586,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1363.5</v>
+        <v>1360.3</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -8725,7 +8725,7 @@
         <v>111.6</v>
       </c>
       <c r="E3">
-        <v>3451</v>
+        <v>3702</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8746,7 +8746,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>2209</v>
+        <v>2329</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -8769,7 +8769,7 @@
         <v>111.6</v>
       </c>
       <c r="E4">
-        <v>4409.3</v>
+        <v>4869.299999999999</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -8813,7 +8813,7 @@
         <v>111.6</v>
       </c>
       <c r="E5">
-        <v>9497.5</v>
+        <v>11533.5</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -8857,7 +8857,7 @@
         <v>111.6</v>
       </c>
       <c r="E6">
-        <v>14483.5</v>
+        <v>17176.5</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -8901,7 +8901,7 @@
         <v>336.6</v>
       </c>
       <c r="E7">
-        <v>15684.5</v>
+        <v>17319.5</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -8922,7 +8922,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>6627</v>
+        <v>9045</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -8945,7 +8945,7 @@
         <v>336.6</v>
       </c>
       <c r="E8">
-        <v>15784.5</v>
+        <v>17319.5</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -8966,7 +8966,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>8187</v>
+        <v>9045</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -8989,7 +8989,7 @@
         <v>336.6</v>
       </c>
       <c r="E9">
-        <v>16810.1</v>
+        <v>19220.1</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -9010,7 +9010,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>8187</v>
+        <v>9045</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -9033,7 +9033,7 @@
         <v>336.6</v>
       </c>
       <c r="E10">
-        <v>17874.1</v>
+        <v>19409.1</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -9054,7 +9054,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>8187</v>
+        <v>9045</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -9077,7 +9077,7 @@
         <v>336.6</v>
       </c>
       <c r="E11">
-        <v>18255.1</v>
+        <v>19790.1</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -9098,7 +9098,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>8187</v>
+        <v>9045</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -9121,7 +9121,7 @@
         <v>336.6</v>
       </c>
       <c r="E12">
-        <v>18715.1</v>
+        <v>19790.1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -9142,7 +9142,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>8661</v>
+        <v>9519</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -9165,7 +9165,7 @@
         <v>336.6</v>
       </c>
       <c r="E13">
-        <v>18715.1</v>
+        <v>19790.1</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -9209,7 +9209,7 @@
         <v>336.6</v>
       </c>
       <c r="E14">
-        <v>19680.1</v>
+        <v>19350.1</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -9530,7 +9530,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>295</v>
+        <v>1180</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -9989,7 +9989,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1592.7</v>
+        <v>2062.4</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -10033,7 +10033,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>2286.4</v>
+        <v>2454.4</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -10071,13 +10071,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>760</v>
+        <v>1150</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -10121,7 +10121,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -10136,7 +10136,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>2557.7</v>
+        <v>3813.7</v>
       </c>
       <c r="M6">
         <v>1354.5</v>
@@ -10165,7 +10165,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -10180,7 +10180,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>3496.7</v>
+        <v>3813.7</v>
       </c>
       <c r="M7">
         <v>1354.5</v>
@@ -10209,7 +10209,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -10253,7 +10253,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -10297,7 +10297,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -10341,7 +10341,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -10385,7 +10385,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>2752.099999999999</v>
+        <v>2752.1</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -10429,7 +10429,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>3637.099999999999</v>
+        <v>3637.1</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -10473,7 +10473,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>3637.099999999999</v>
+        <v>3637.1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -10589,7 +10589,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>110</v>
+        <v>440</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -10633,7 +10633,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -10677,7 +10677,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -10721,7 +10721,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -10765,10 +10765,10 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="M6">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -10809,7 +10809,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="M7">
         <v>1000</v>
@@ -10853,7 +10853,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="M8">
         <v>1000</v>
@@ -10897,7 +10897,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="M9">
         <v>1000</v>
@@ -10941,7 +10941,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>330</v>
+        <v>440</v>
       </c>
       <c r="M10">
         <v>1940</v>
@@ -11117,7 +11117,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <v>1940</v>
@@ -11203,7 +11203,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>23</v>
+        <v>297</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -11218,7 +11218,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>539</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -11247,7 +11247,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>46</v>
+        <v>297</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -11262,7 +11262,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>539</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -11291,7 +11291,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>46</v>
+        <v>297</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -11306,7 +11306,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>748</v>
+        <v>259</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -11350,7 +11350,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>996</v>
+        <v>1351</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -11394,7 +11394,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1301</v>
+        <v>1351</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -12046,7 +12046,7 @@
         <v>20</v>
       </c>
       <c r="E7">
-        <v>9852.799999999999</v>
+        <v>9852.799999999997</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -12090,7 +12090,7 @@
         <v>20</v>
       </c>
       <c r="E8">
-        <v>9852.799999999999</v>
+        <v>9852.799999999997</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -12134,7 +12134,7 @@
         <v>20</v>
       </c>
       <c r="E9">
-        <v>9852.799999999999</v>
+        <v>9852.799999999997</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -12354,7 +12354,7 @@
         <v>20</v>
       </c>
       <c r="E14">
-        <v>9673</v>
+        <v>9672.999999999998</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -12570,7 +12570,7 @@
         <v>638</v>
       </c>
       <c r="N4">
-        <v>1503</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -13010,7 +13010,7 @@
         <v>8414</v>
       </c>
       <c r="N14">
-        <v>2173</v>
+        <v>1503</v>
       </c>
     </row>
   </sheetData>
@@ -13090,7 +13090,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>3547</v>
+        <v>3462</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -13111,7 +13111,7 @@
         <v>1340</v>
       </c>
       <c r="N2">
-        <v>252</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -13134,7 +13134,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>3547</v>
+        <v>3462</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -13152,10 +13152,10 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>2660</v>
       </c>
       <c r="N3">
-        <v>252</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -13178,7 +13178,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>3547</v>
+        <v>3462</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -13196,10 +13196,10 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>2560</v>
+        <v>3220</v>
       </c>
       <c r="N4">
-        <v>352</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -13222,7 +13222,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>3547</v>
+        <v>3462</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -13240,10 +13240,10 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2560</v>
+        <v>3220</v>
       </c>
       <c r="N5">
-        <v>862</v>
+        <v>878</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -13266,7 +13266,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>3619</v>
+        <v>3606</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -13284,10 +13284,10 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>5280</v>
+        <v>5940</v>
       </c>
       <c r="N6">
-        <v>2328</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -13310,7 +13310,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>3691</v>
+        <v>3606</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -13331,7 +13331,7 @@
         <v>5940</v>
       </c>
       <c r="N7">
-        <v>4379</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -13354,7 +13354,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>3691</v>
+        <v>3606</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -13375,7 +13375,7 @@
         <v>11318</v>
       </c>
       <c r="N8">
-        <v>4379</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -13398,7 +13398,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>10320</v>
+        <v>10235</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -13419,7 +13419,7 @@
         <v>12638</v>
       </c>
       <c r="N9">
-        <v>4379</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -13442,7 +13442,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>19534</v>
+        <v>19449</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -13463,7 +13463,7 @@
         <v>12638</v>
       </c>
       <c r="N10">
-        <v>4379</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -13507,7 +13507,7 @@
         <v>12638</v>
       </c>
       <c r="N11">
-        <v>4379</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -13530,7 +13530,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>30014</v>
+        <v>30439</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -13568,7 +13568,7 @@
         <v>2035</v>
       </c>
       <c r="E13">
-        <v>19744</v>
+        <v>20724</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -13734,7 +13734,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1899</v>
+        <v>1213</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -13778,7 +13778,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1899</v>
+        <v>1213</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -13822,7 +13822,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>2595</v>
+        <v>2817</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -13866,7 +13866,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>3515</v>
+        <v>3507</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -13910,7 +13910,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>3963</v>
+        <v>3507</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -13954,7 +13954,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>3963</v>
+        <v>3507</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -13998,10 +13998,10 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>3963</v>
+        <v>3507</v>
       </c>
       <c r="M8">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -14042,7 +14042,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>4193</v>
+        <v>3507</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -14086,7 +14086,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>4193</v>
+        <v>3507</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -14130,7 +14130,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>4193</v>
+        <v>3507</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -14174,7 +14174,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>4193</v>
+        <v>3507</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -14342,13 +14342,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -14369,7 +14369,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -14386,13 +14386,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -14413,7 +14413,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -14430,13 +14430,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -14457,7 +14457,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -14474,13 +14474,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -14501,7 +14501,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -14518,13 +14518,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -14545,7 +14545,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -14562,13 +14562,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -14589,7 +14589,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -14606,13 +14606,13 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -14633,7 +14633,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -14650,13 +14650,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -14677,7 +14677,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -14694,13 +14694,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -14721,7 +14721,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -14738,13 +14738,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -14765,7 +14765,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -14782,13 +14782,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -14809,7 +14809,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -14826,13 +14826,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -14853,7 +14853,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -14870,13 +14870,13 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>343.5</v>
+        <v>330</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1456.23</v>
+        <v>112</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -14897,7 +14897,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>360.5</v>
+        <v>740</v>
       </c>
     </row>
   </sheetData>
@@ -14992,7 +14992,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>2531</v>
+        <v>1850</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -15036,7 +15036,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>2531</v>
+        <v>1850</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -15080,7 +15080,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>2718</v>
+        <v>2780</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -15103,7 +15103,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>547</v>
+        <v>922</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -15124,7 +15124,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>3819</v>
+        <v>3508</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -15168,7 +15168,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>4957</v>
+        <v>4276</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -15215,7 +15215,7 @@
         <v>5750</v>
       </c>
       <c r="M7">
-        <v>470</v>
+        <v>1880</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -15644,7 +15644,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>147</v>
+        <v>787</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -15688,7 +15688,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>411</v>
+        <v>1051</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -15732,7 +15732,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>411</v>
+        <v>1051</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -15759,7 +15759,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>260</v>
+        <v>520</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -15776,7 +15776,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1417</v>
+        <v>2057</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -16344,7 +16344,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1380</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -16858,13 +16858,13 @@
         <v>920</v>
       </c>
       <c r="E2">
-        <v>661</v>
+        <v>766</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>550</v>
+        <v>390</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -16902,13 +16902,13 @@
         <v>920</v>
       </c>
       <c r="E3">
-        <v>661</v>
+        <v>766</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>550</v>
+        <v>390</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -16946,13 +16946,13 @@
         <v>920</v>
       </c>
       <c r="E4">
-        <v>661</v>
+        <v>766</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>550</v>
+        <v>390</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -16990,13 +16990,13 @@
         <v>920</v>
       </c>
       <c r="E5">
-        <v>1806</v>
+        <v>2504</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>550</v>
+        <v>390</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -17034,13 +17034,13 @@
         <v>920</v>
       </c>
       <c r="E6">
-        <v>2281</v>
+        <v>2744</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>550</v>
+        <v>390</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -17078,13 +17078,13 @@
         <v>920</v>
       </c>
       <c r="E7">
-        <v>2436</v>
+        <v>2899</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>904</v>
+        <v>744</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -17122,13 +17122,13 @@
         <v>920</v>
       </c>
       <c r="E8">
-        <v>2676</v>
+        <v>2899</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>904</v>
+        <v>744</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -17166,7 +17166,7 @@
         <v>920</v>
       </c>
       <c r="E9">
-        <v>3241</v>
+        <v>3464</v>
       </c>
       <c r="F9">
         <v>0</v>

</xml_diff>

<commit_message>
a lot of preprocessing
</commit_message>
<xml_diff>
--- a/grouped.xlsx
+++ b/grouped.xlsx
@@ -25,15 +25,15 @@
     <sheet name="LI" sheetId="16" r:id="rId16"/>
     <sheet name="LU" sheetId="17" r:id="rId17"/>
     <sheet name="MT" sheetId="18" r:id="rId18"/>
-    <sheet name="NT" sheetId="19" r:id="rId19"/>
+    <sheet name="NL" sheetId="19" r:id="rId19"/>
     <sheet name="NO" sheetId="20" r:id="rId20"/>
     <sheet name="PL" sheetId="21" r:id="rId21"/>
     <sheet name="PT" sheetId="22" r:id="rId22"/>
     <sheet name="RO" sheetId="23" r:id="rId23"/>
     <sheet name="SK" sheetId="24" r:id="rId24"/>
-    <sheet name="SO" sheetId="25" r:id="rId25"/>
+    <sheet name="SI" sheetId="25" r:id="rId25"/>
     <sheet name="ES" sheetId="26" r:id="rId26"/>
-    <sheet name="SW" sheetId="27" r:id="rId27"/>
+    <sheet name="SE" sheetId="27" r:id="rId27"/>
     <sheet name="UK" sheetId="28" r:id="rId28"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
added choosing data source by type
</commit_message>
<xml_diff>
--- a/grouped.xlsx
+++ b/grouped.xlsx
@@ -1157,7 +1157,7 @@
         <v>1.664</v>
       </c>
       <c r="M2">
-        <v>1.275</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0.7292000000000001</v>
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>3.701400000000001</v>
+        <v>3.7014</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>4.065700000000001</v>
+        <v>4.0657</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1324,7 +1324,7 @@
         <v>0.3210000000000001</v>
       </c>
       <c r="J6">
-        <v>0.9881799999999994</v>
+        <v>0.9881800000000003</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1333,10 +1333,10 @@
         <v>4.063499999999998</v>
       </c>
       <c r="M6">
-        <v>1.402</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>1.330899999999999</v>
+        <v>1.3309</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1377,10 +1377,10 @@
         <v>5.571300000000001</v>
       </c>
       <c r="M7">
-        <v>6.58</v>
+        <v>2.648</v>
       </c>
       <c r="N7">
-        <v>0.09359999999999946</v>
+        <v>0.09360000000000035</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1412,7 +1412,7 @@
         <v>0.3334999999999999</v>
       </c>
       <c r="J8">
-        <v>0.2111910000000004</v>
+        <v>0.2111909999999995</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1421,10 +1421,10 @@
         <v>1.1111</v>
       </c>
       <c r="M8">
-        <v>10.942</v>
+        <v>5.476</v>
       </c>
       <c r="N8">
-        <v>0.04140000000000121</v>
+        <v>0.04140000000000033</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1447,16 +1447,16 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1.752009999999995</v>
+        <v>1.752009999999999</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.07580000000000031</v>
+        <v>0.07580000000000009</v>
       </c>
       <c r="J9">
-        <v>0.510978999999999</v>
+        <v>0.5109789999999998</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1485,22 +1485,22 @@
         <v>0.03749999999999999</v>
       </c>
       <c r="E10">
-        <v>0.5953999999999979</v>
+        <v>0.595400000000005</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>5.829400000000007</v>
+        <v>5.829400000000003</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.1824999999999997</v>
+        <v>0.1824999999999999</v>
       </c>
       <c r="J10">
-        <v>0.617020000000001</v>
+        <v>0.6170200000000001</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1526,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.5754933999999999</v>
+        <v>0.5754934</v>
       </c>
       <c r="E11">
         <v>0.2549999999999955</v>
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.07520000000000038</v>
+        <v>0.07520000000000016</v>
       </c>
       <c r="J11">
         <v>0.5482499999999995</v>
@@ -1573,7 +1573,7 @@
         <v>0.17175</v>
       </c>
       <c r="E12">
-        <v>0.3736000000000104</v>
+        <v>0.3736000000000033</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1585,10 +1585,10 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.4294999999999993</v>
+        <v>0.4295</v>
       </c>
       <c r="J12">
-        <v>0.1690149999999999</v>
+        <v>0.1690150000000008</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0.4079999999999995</v>
+        <v>0.4080000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.01510000000000011</v>
+        <v>0.0151</v>
       </c>
       <c r="E13">
         <v>10.37669999999999</v>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.1779700000000002</v>
+        <v>0.1779699999999997</v>
       </c>
       <c r="J13">
         <v>0.6781499999999996</v>
@@ -1644,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0.1632999999999996</v>
+        <v>0.1632999999999978</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1.333160999999999</v>
+        <v>1.333161</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3026,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.6078000000000001</v>
+        <v>0.6078</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.8409999999999995</v>
+        <v>0.8409999999999999</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3202,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.8640000000000001</v>
+        <v>0.8640000000000003</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -7913,7 +7913,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.8248000000000011</v>
+        <v>0.8248000000000002</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -8813,7 +8813,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>6.664200000000001</v>
+        <v>6.6642</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -8901,7 +8901,7 @@
         <v>0.225</v>
       </c>
       <c r="E7">
-        <v>0.1430000000000007</v>
+        <v>0.1429999999999971</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -9039,7 +9039,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.1289</v>
+        <v>0.1288999999999998</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -10077,7 +10077,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.2977000000000003</v>
+        <v>0.2976999999999999</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -10429,7 +10429,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.8849999999999993</v>
+        <v>0.8849999999999998</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -10812,7 +10812,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -10944,7 +10944,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>1.88</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -11832,7 +11832,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.7645999999999999</v>
+        <v>0.7646000000000001</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -11914,7 +11914,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.6454000000000001</v>
+        <v>0.6454</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -12002,7 +12002,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>3.315499999999999</v>
+        <v>3.3155</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -12222,13 +12222,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>6.233930000000003</v>
+        <v>6.233930000000001</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>9.879599999999998</v>
+        <v>9.879600000000002</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -12479,7 +12479,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2.511</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>2.239</v>
@@ -12611,7 +12611,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0.8649999999999998</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>0.6699999999999999</v>
@@ -12655,7 +12655,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1.862000000000001</v>
+        <v>1.862</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -12699,7 +12699,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>5.687</v>
+        <v>5.686999999999999</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -13284,7 +13284,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>4.801</v>
+        <v>2.72</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -13328,7 +13328,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>3.506</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0.7180000000000001</v>
@@ -13372,7 +13372,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>7.882</v>
+        <v>5.377999999999999</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -13416,7 +13416,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>2.542999999999999</v>
+        <v>1.32</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -14542,7 +14542,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1.035</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>

</xml_diff>

<commit_message>
bugfix, files for separate dbs
</commit_message>
<xml_diff>
--- a/grouped.xlsx
+++ b/grouped.xlsx
@@ -17,8 +17,8 @@
     <sheet name="FI" sheetId="8" r:id="rId8"/>
     <sheet name="FR" sheetId="9" r:id="rId9"/>
     <sheet name="DE" sheetId="10" r:id="rId10"/>
-    <sheet name="HL" sheetId="11" r:id="rId11"/>
-    <sheet name="IR" sheetId="12" r:id="rId12"/>
+    <sheet name="EL" sheetId="11" r:id="rId11"/>
+    <sheet name="IE" sheetId="12" r:id="rId12"/>
     <sheet name="HU" sheetId="13" r:id="rId13"/>
     <sheet name="IT" sheetId="14" r:id="rId14"/>
     <sheet name="LV" sheetId="15" r:id="rId15"/>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.4786999999999995</v>
+        <v>0.08369999999999989</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.925</v>
+        <v>0.4649999999999999</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>1.670000000000001</v>
+        <v>0.8319999999999999</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1221,13 +1221,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.416189999999999</v>
+        <v>3.056189999999999</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.03189999999999982</v>
+        <v>0.002900000000000125</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1309,13 +1309,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1.671600000000001</v>
+        <v>2.428600000000001</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1.451700000000001</v>
+        <v>1.571700000000001</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1353,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>9.193099999999998</v>
+        <v>8.380099999999997</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.7132999999999985</v>
+        <v>0.3613</v>
       </c>
       <c r="M7">
         <v>2.648</v>
@@ -1418,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.6461000000000006</v>
+        <v>0.6460999999999988</v>
       </c>
       <c r="M8">
         <v>5.476</v>
@@ -1441,13 +1441,13 @@
         <v>0.03129999999999999</v>
       </c>
       <c r="E9">
-        <v>2.020400000000006</v>
+        <v>1.687400000000004</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.9992099999999997</v>
+        <v>0.9992099999999988</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1456,7 +1456,7 @@
         <v>0.005100000000000104</v>
       </c>
       <c r="J9">
-        <v>0.3677790000000001</v>
+        <v>0.3774790000000006</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1485,22 +1485,22 @@
         <v>0.08640000000000003</v>
       </c>
       <c r="E10">
-        <v>0.259400000000003</v>
+        <v>0.2593999999999994</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>4.239100000000003</v>
+        <v>4.118400000000002</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.1040999999999999</v>
+        <v>0.1108</v>
       </c>
       <c r="J10">
-        <v>0.591219999999999</v>
+        <v>0.5912199999999999</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1535,16 +1535,16 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1.753159</v>
+        <v>1.753159000000002</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.04449999999999998</v>
+        <v>0.07519999999999971</v>
       </c>
       <c r="J11">
-        <v>0.4382500000000009</v>
+        <v>0.4382499999999983</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1570,16 +1570,16 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.3057499999999999</v>
+        <v>0.26985</v>
       </c>
       <c r="E12">
-        <v>0.05059999999999576</v>
+        <v>0.05059999999999931</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>2.987100000000003</v>
+        <v>2.987100000000002</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1614,25 +1614,25 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.01510000000000011</v>
+        <v>0.01509999999999989</v>
       </c>
       <c r="E13">
-        <v>8.557699999999997</v>
+        <v>7.831700000000001</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2.482799999999994</v>
+        <v>2.482799999999997</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.1589599999999998</v>
+        <v>0.15896</v>
       </c>
       <c r="J13">
-        <v>0.4084499999999984</v>
+        <v>0.4084500000000002</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1667,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1.567500000000003</v>
+        <v>1.567499999999999</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1.294461000000001</v>
+        <v>1.294461</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -2252,7 +2252,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>1.302</v>
+        <v>0.8649999999999993</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -3887,7 +3887,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.114</v>
+        <v>0.134</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -3931,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -3975,7 +3975,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.109</v>
+        <v>0.08900000000000002</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -4007,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>4.428000000000001</v>
+        <v>3.798000000000002</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -4019,7 +4019,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0.424</v>
+        <v>0.352</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -4063,7 +4063,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0.573</v>
+        <v>0.4480000000000001</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>13.608</v>
+        <v>12.002</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -4107,7 +4107,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0.05400000000000005</v>
+        <v>0.05399999999999983</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -4139,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>4.369</v>
+        <v>3.568999999999996</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -7284,7 +7284,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>3.982999999999999</v>
+        <v>2.671999999999999</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -7781,7 +7781,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1.172</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -7825,7 +7825,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.3763999999999994</v>
+        <v>0.3763999999999998</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -7913,7 +7913,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>1.2298</v>
+        <v>0.8247999999999998</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -9162,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.205</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -9756,7 +9756,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.652</v>
+        <v>0.8260000000000001</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -10429,7 +10429,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>1.745</v>
+        <v>0.8850000000000002</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -12228,7 +12228,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>13.189496</v>
+        <v>11.978166</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -12272,7 +12272,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>20.51955999999998</v>
+        <v>18.88164</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -12316,7 +12316,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>4.333050000000007</v>
+        <v>4.333049999999993</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -15908,7 +15908,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1.159</v>
+        <v>0.7869999999999999</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -17707,7 +17707,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2.38</v>
+        <v>1.785</v>
       </c>
       <c r="F7">
         <v>0</v>

</xml_diff>

<commit_message>
entsoe comparison and report added
</commit_message>
<xml_diff>
--- a/grouped.xlsx
+++ b/grouped.xlsx
@@ -13,7 +13,7 @@
     <sheet name="CH" sheetId="4" r:id="rId4"/>
     <sheet name="CZ" sheetId="5" r:id="rId5"/>
     <sheet name="DK" sheetId="6" r:id="rId6"/>
-    <sheet name="ET" sheetId="7" r:id="rId7"/>
+    <sheet name="EE" sheetId="7" r:id="rId7"/>
     <sheet name="FI" sheetId="8" r:id="rId8"/>
     <sheet name="FR" sheetId="9" r:id="rId9"/>
     <sheet name="DE" sheetId="10" r:id="rId10"/>
@@ -22,26 +22,25 @@
     <sheet name="HU" sheetId="13" r:id="rId13"/>
     <sheet name="IT" sheetId="14" r:id="rId14"/>
     <sheet name="LV" sheetId="15" r:id="rId15"/>
-    <sheet name="LI" sheetId="16" r:id="rId16"/>
+    <sheet name="LT" sheetId="16" r:id="rId16"/>
     <sheet name="LU" sheetId="17" r:id="rId17"/>
-    <sheet name="MT" sheetId="18" r:id="rId18"/>
-    <sheet name="NL" sheetId="19" r:id="rId19"/>
-    <sheet name="NO" sheetId="20" r:id="rId20"/>
-    <sheet name="PL" sheetId="21" r:id="rId21"/>
-    <sheet name="PT" sheetId="22" r:id="rId22"/>
-    <sheet name="RO" sheetId="23" r:id="rId23"/>
-    <sheet name="SK" sheetId="24" r:id="rId24"/>
-    <sheet name="SI" sheetId="25" r:id="rId25"/>
-    <sheet name="ES" sheetId="26" r:id="rId26"/>
-    <sheet name="SE" sheetId="27" r:id="rId27"/>
-    <sheet name="UK" sheetId="28" r:id="rId28"/>
+    <sheet name="NL" sheetId="18" r:id="rId18"/>
+    <sheet name="NO" sheetId="19" r:id="rId19"/>
+    <sheet name="PL" sheetId="20" r:id="rId20"/>
+    <sheet name="PT" sheetId="21" r:id="rId21"/>
+    <sheet name="RO" sheetId="22" r:id="rId22"/>
+    <sheet name="SK" sheetId="23" r:id="rId23"/>
+    <sheet name="SI" sheetId="24" r:id="rId24"/>
+    <sheet name="ES" sheetId="25" r:id="rId25"/>
+    <sheet name="SE" sheetId="26" r:id="rId26"/>
+    <sheet name="UK" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="14">
   <si>
     <t>year</t>
   </si>
@@ -510,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.4012</v>
+        <v>0.2911450105734993</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -531,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.15</v>
+        <v>0.07613636363636363</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -598,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.4708</v>
+        <v>0.3416527192871473</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -642,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1.24</v>
+        <v>0.89984998282936</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -724,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.715</v>
+        <v>0.1922295081967213</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -768,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0.2</v>
+        <v>0.05377049180327868</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -795,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0.246</v>
+        <v>0.1248636363636364</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -818,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1.598</v>
+        <v>1.159645381097836</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -862,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.04700000000000015</v>
+        <v>0.03410721709111295</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -906,13 +905,13 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.08369999999999989</v>
+        <v>0.06073987384098171</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.395</v>
+        <v>0.2866457606593525</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -950,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.4649999999999999</v>
+        <v>0.3374437435610099</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -994,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.8319999999999999</v>
+        <v>0.6037703110596995</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1133,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1.52932</v>
+        <v>1.091761329511611</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1154,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1.551</v>
+        <v>1.45909117701958</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1177,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2.007000000000001</v>
+        <v>1.432770766307774</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1198,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>6.7425</v>
+        <v>6.342954391395561</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1221,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>3.056189999999999</v>
+        <v>2.181773636413628</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1242,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1.535</v>
+        <v>1.444039301563543</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1265,7 +1264,7 @@
         <v>0.052</v>
       </c>
       <c r="E5">
-        <v>1.15056</v>
+        <v>0.8213695729362592</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1286,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>2.894</v>
+        <v>2.722507973110679</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1309,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2.428600000000001</v>
+        <v>1.733745432513732</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1330,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.05949999999999989</v>
+        <v>0.05597416185213721</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1353,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>8.380099999999997</v>
+        <v>5.982442600266949</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1374,10 +1373,10 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.3613</v>
+        <v>0.3398901626416338</v>
       </c>
       <c r="M7">
-        <v>2.648</v>
+        <v>2.644740521910389</v>
       </c>
       <c r="N7">
         <v>0.1594000000000007</v>
@@ -1397,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>3.077900000000007</v>
+        <v>2.19727211839497</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1418,10 +1417,10 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.6460999999999988</v>
+        <v>0.60781354575909</v>
       </c>
       <c r="M8">
-        <v>5.476</v>
+        <v>5.469259478089612</v>
       </c>
       <c r="N8">
         <v>0.04140000000000033</v>
@@ -1441,7 +1440,7 @@
         <v>0.03129999999999999</v>
       </c>
       <c r="E9">
-        <v>1.687400000000004</v>
+        <v>1.20461255160326</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1462,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0.1593</v>
+        <v>0.1498602350091676</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1485,7 +1484,7 @@
         <v>0.08640000000000003</v>
       </c>
       <c r="E10">
-        <v>0.2593999999999994</v>
+        <v>0.185182230583077</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1506,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>5.662999999999997</v>
+        <v>5.327423169221067</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1550,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.9672200000000011</v>
+        <v>0.9099046861617532</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1573,7 +1572,7 @@
         <v>0.26985</v>
       </c>
       <c r="E12">
-        <v>0.05059999999999931</v>
+        <v>0.03612267103894985</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1594,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0.09479999999999933</v>
+        <v>0.08918236207701816</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1617,7 +1616,7 @@
         <v>0.01509999999999989</v>
       </c>
       <c r="E13">
-        <v>7.831700000000001</v>
+        <v>5.590947090429791</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1638,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1.720300000000002</v>
+        <v>1.618358834188772</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1768,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.588</v>
+        <v>1.364722300140253</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2003,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1.674</v>
+        <v>1.337767530306632</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -2047,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.5459999999999998</v>
+        <v>0.436332778702163</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -2091,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0.5110000000000001</v>
+        <v>0.4083627287853578</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -2120,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.6839999999999997</v>
+        <v>0.5878274894810657</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -2135,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.3420000000000001</v>
+        <v>0.2733073449013549</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -2164,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1.023</v>
+        <v>0.879163043478261</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -2179,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.2889999999999997</v>
+        <v>0.230952697884478</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -2208,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.544</v>
+        <v>1.326908835904629</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2252,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.8649999999999993</v>
+        <v>0.7433783309957919</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2267,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0.8450000000000002</v>
+        <v>0.6752769194200144</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3041,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.962</v>
+        <v>0.8195719120135363</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -3085,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0.22</v>
+        <v>0.1874280879864636</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -3649,13 +3648,13 @@
         <v>0.571</v>
       </c>
       <c r="E2">
-        <v>0.143</v>
+        <v>0.1421601409553641</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>12.5544</v>
+        <v>10.27220785678001</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3667,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.028</v>
+        <v>0.01938804780876494</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -3676,7 +3675,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>9.823</v>
+        <v>2.341590372388737</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3693,13 +3692,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.3150000000000001</v>
+        <v>0.3131499608457322</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.7530000000000001</v>
+        <v>0.6161164624478551</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -3720,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6129999999999995</v>
+        <v>0.1461259185864089</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3737,13 +3736,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1.292</v>
+        <v>1.284411902897416</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1.079000000000001</v>
+        <v>0.8828547981158511</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3781,13 +3780,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.593</v>
+        <v>0.5895172278778387</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1.488</v>
+        <v>1.217505041331219</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3808,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.266</v>
+        <v>0.3017869705226653</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3831,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.5760000000000023</v>
+        <v>0.4712922740636997</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3852,7 +3851,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.3520000000000003</v>
+        <v>0.08390917347865584</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -3875,7 +3874,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.3999999999999986</v>
+        <v>0.3272863014331223</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3887,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.134</v>
+        <v>0.09278565737051794</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -3931,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0.15</v>
+        <v>0.1038645418326693</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -3957,13 +3956,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>2.954</v>
+        <v>2.936650743931088</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.3719999999999999</v>
+        <v>0.3043762603328047</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3975,7 +3974,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.08900000000000002</v>
+        <v>0.06162629482071715</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -4001,13 +4000,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.5200000000000005</v>
+        <v>0.5169459671104155</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>3.798000000000002</v>
+        <v>3.107583432107509</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -4019,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0.352</v>
+        <v>0.2437354581673307</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -4051,7 +4050,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>15.379</v>
+        <v>12.58334007435001</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -4063,7 +4062,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0.4480000000000001</v>
+        <v>0.3102087649402391</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -4072,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.05700000000000038</v>
+        <v>0.01358756502353242</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -4089,13 +4088,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1.845</v>
+        <v>1.834164056382145</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>12.002</v>
+        <v>9.820225474500873</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -4107,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0.05399999999999983</v>
+        <v>0.03739123505976084</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -4139,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>3.568999999999996</v>
+        <v>2.920212024537041</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -4913,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>3.535</v>
+        <v>1.716584362139918</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -5089,7 +5088,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.1099999999999999</v>
+        <v>0.05341563786008224</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -5542,7 +5541,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.385</v>
+        <v>0.081</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -6165,13 +6164,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>3.171819947400365</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>2.486</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -6303,7 +6302,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.8689999999999998</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -6347,7 +6346,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.5739999999999998</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -6479,7 +6478,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1.763</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -6523,7 +6522,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>4.183</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -6567,7 +6566,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.8399999999999999</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -6611,7 +6610,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1.848000000000001</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -6649,13 +6648,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1.490180052599636</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2.671999999999999</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -6794,13 +6793,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3.363</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2.486</v>
+        <v>0.642</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -6932,7 +6931,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.8689999999999998</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -6976,7 +6975,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.5739999999999998</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -7108,7 +7107,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1.763</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -7152,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>4.183</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -7196,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.8399999999999999</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -7240,7 +7239,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.848000000000001</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -7278,13 +7277,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1.58</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2.671999999999999</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -7450,7 +7449,7 @@
         <v>0.481</v>
       </c>
       <c r="N2">
-        <v>0.4964</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -8049,16 +8048,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.1116</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2.1298</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2.2975</v>
+        <v>1.4112</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -8073,7 +8072,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.2074399596367306</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -8096,7 +8095,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1.4622</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8117,7 +8116,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1.280791120080726</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -8140,7 +8139,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1.1673</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -8161,7 +8160,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1.070768920282543</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -8184,13 +8183,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>6.664200000000001</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.07699999999999996</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -8228,7 +8227,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5.643000000000001</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -8269,10 +8268,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.225</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.1429999999999971</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -8293,7 +8292,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>4.710006054490414</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -8360,7 +8359,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1.900600000000008</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -8404,13 +8403,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.1890000000000001</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.1289000000000002</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -8448,13 +8447,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.3810000000000002</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.4179999999999999</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -8489,7 +8488,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -8513,7 +8512,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>0.4079939455095864</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -8533,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.205</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -8586,7 +8585,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.4849999999999999</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -8607,7 +8606,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>0.359</v>
       </c>
     </row>
   </sheetData>
@@ -8678,16 +8677,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.1116</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>2.1298</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.4112</v>
+        <v>1.826</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -8702,7 +8701,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.241</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -8725,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1.4622</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8746,7 +8745,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1.488</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -8769,7 +8768,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1.1673</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -8790,7 +8789,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1.244</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -8813,13 +8812,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>6.664200000000001</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.07699999999999996</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -8857,7 +8856,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>5.643000000000001</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -8898,10 +8897,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.225</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.1429999999999971</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -8922,7 +8921,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>5.472</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -8986,10 +8985,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="E9">
-        <v>1.900600000000008</v>
+        <v>0.5760000000000001</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -9030,16 +9029,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.01899999999999999</v>
       </c>
       <c r="E10">
-        <v>0.1890000000000001</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.1289000000000002</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -9074,16 +9073,16 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.2329</v>
       </c>
       <c r="E11">
-        <v>0.3810000000000002</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.4179999999999999</v>
+        <v>1.176</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -9118,7 +9117,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.01000000000000001</v>
+        <v>0.101</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -9127,7 +9126,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.8260000000000001</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -9139,10 +9138,10 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="L12">
-        <v>0.4740000000000002</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -9162,7 +9161,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.205</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -9215,7 +9214,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.4849999999999999</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -9236,7 +9235,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>1.015</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9316,7 +9315,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.826</v>
+        <v>0.897859531772575</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -9331,10 +9330,10 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.4337548333226284</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -9360,7 +9359,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.5276566332218507</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -9404,7 +9403,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.2709476031215161</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -9442,13 +9441,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.2057681159420292</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -9507,7 +9506,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>2.073764960284326</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -9595,7 +9594,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.5634802063930462</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -9615,10 +9614,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.5760000000000001</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -9659,7 +9658,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.01899999999999999</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -9703,7 +9702,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.2329</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -9712,7 +9711,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1.176</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -9747,7 +9746,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.101</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -9756,7 +9755,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.8260000000000001</v>
+        <v>0.1520624303232997</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -9768,7 +9767,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -9800,7 +9799,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.6117056856187292</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -9945,7 +9944,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.299</v>
+        <v>0.298</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -9960,10 +9959,10 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.6597000000000001</v>
+        <v>0.33</v>
       </c>
       <c r="M2">
-        <v>1.3545</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -9989,7 +9988,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.7634000000000003</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -10033,7 +10032,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.3919999999999999</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -10071,13 +10070,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.9999999999999999</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.2977000000000003</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -10136,7 +10135,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>3.154</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -10224,7 +10223,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.8570000000000002</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -10297,7 +10296,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.158</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -10315,7 +10314,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -10385,7 +10384,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.2199999999999998</v>
+        <v>0.4196</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -10429,7 +10428,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.8850000000000002</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -10574,13 +10573,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.298</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.053</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -10589,7 +10588,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -10809,7 +10808,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>0.04999999999999999</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -10926,7 +10925,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.158</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -10944,7 +10943,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0.9399999999999999</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -11014,7 +11013,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.4196</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -11073,7 +11072,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -11194,22 +11193,22 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.03124145615252358</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.9559728670694533</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.053</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -11224,7 +11223,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.002825140233798355</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -11285,7 +11284,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.2168089871057927</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -11312,7 +11311,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.09486820905094874</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -11329,7 +11328,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.3585041075911092</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -11356,7 +11355,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>0.1583879557826125</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -11373,7 +11372,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.113774708319268</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -11400,7 +11399,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.02718138047443245</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -11417,7 +11416,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.371567111022995</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -11438,7 +11437,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.04999999999999999</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -11485,10 +11484,10 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>3.0404</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>0.1658957659539316</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -11505,13 +11504,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.02821808942808569</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.06619672903549409</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -11532,7 +11531,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>0.04167611558646402</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -11549,13 +11548,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.2194786199234713</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.05005459498621786</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -11576,7 +11575,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>0.1119110440826019</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -11593,13 +11592,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2.094161836052704</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>9.849880857691524</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -11620,7 +11619,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>0.02239100206549814</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -11637,13 +11636,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>3.634575916324279</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>15.52674294193474</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -11664,7 +11663,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>0.1441633747054377</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -11681,13 +11680,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.1456691680797723</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>3.563152009282573</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -11702,13 +11701,13 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0.6000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>0.05470001206427444</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -11823,16 +11822,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.02</v>
+        <v>0.405</v>
       </c>
       <c r="E2">
-        <v>0.093</v>
+        <v>0.13</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.162532</v>
+        <v>0.708</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -11853,7 +11852,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.016</v>
+        <v>1.569</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -11911,10 +11910,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.01999999999999996</v>
       </c>
       <c r="E4">
-        <v>0.6454000000000001</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -11941,7 +11940,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.53728</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -11958,7 +11957,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1.0672</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -11985,7 +11984,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8970199999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -12002,13 +12001,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>3.315499999999999</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.639</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -12026,10 +12025,10 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1.862</v>
       </c>
       <c r="N6">
-        <v>0.1539400000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -12046,7 +12045,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4.082900000000001</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -12070,7 +12069,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>5.686999999999999</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -12114,10 +12113,10 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>3.0404</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>0.9395399999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -12134,13 +12133,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.08399999999999963</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.08050000000000002</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -12161,7 +12160,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0.2360299999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -12175,16 +12174,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.03870000000000001</v>
       </c>
       <c r="E10">
-        <v>0.6533470000000001</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.0608700000000002</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -12205,7 +12204,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.6338010000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -12222,13 +12221,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>6.233930000000004</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>11.978166</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -12249,7 +12248,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.1268100000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -12266,13 +12265,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>10.819456</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>18.88164</v>
+        <v>0.25</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -12293,7 +12292,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0.8164599999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -12310,13 +12309,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0.4336300000000008</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>4.333049999999993</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -12337,7 +12336,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0.3097899999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -12351,7 +12350,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -12452,16 +12451,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.405</v>
+        <v>1.6837</v>
       </c>
       <c r="E2">
-        <v>0.13</v>
+        <v>2.077567065245646</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.708</v>
+        <v>6.206300000000001</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -12482,7 +12481,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1.569</v>
+        <v>0.4234</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -12540,10 +12539,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.01999999999999996</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2.426909279958409</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -12570,7 +12569,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.26</v>
+        <v>0.09999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -12584,10 +12583,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.934999999999998</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1.872322589030413</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -12614,7 +12613,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>0.7270000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -12637,7 +12636,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.639</v>
+        <v>0.1439999999999992</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -12655,7 +12654,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1.862</v>
+        <v>2.370830324909747</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -12699,10 +12698,10 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>5.686999999999999</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>0.718</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -12719,7 +12718,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.9172010657655317</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -12743,7 +12742,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>4.687619664472287</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -12769,7 +12768,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>6.628999999999999</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -12787,636 +12786,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10">
-        <v>2020</v>
-      </c>
-      <c r="B10">
-        <v>2000</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0.03870000000000001</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11">
-        <v>2020</v>
-      </c>
-      <c r="B11">
-        <v>2005</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
-        <v>2010</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0.25</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13">
-        <v>2020</v>
-      </c>
-      <c r="B13">
-        <v>2015</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14">
-        <v>2020</v>
-      </c>
-      <c r="B14">
-        <v>2020</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0.12</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2">
-        <v>2020</v>
-      </c>
-      <c r="B2">
-        <v>1960</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1.6837</v>
-      </c>
-      <c r="E2">
-        <v>4.383</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>6.206300000000001</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0.4234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>2020</v>
-      </c>
-      <c r="B3">
-        <v>1965</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4">
-        <v>2020</v>
-      </c>
-      <c r="B4">
-        <v>1970</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>5.12</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0.09999999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5">
-        <v>2020</v>
-      </c>
-      <c r="B5">
-        <v>1975</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1.934999999999998</v>
-      </c>
-      <c r="E5">
-        <v>3.949999999999999</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0.7270000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6">
-        <v>2020</v>
-      </c>
-      <c r="B6">
-        <v>1980</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0.1439999999999992</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>2.72</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7">
-        <v>2020</v>
-      </c>
-      <c r="B7">
-        <v>1985</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0.718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8">
-        <v>2020</v>
-      </c>
-      <c r="B8">
-        <v>1990</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1.935</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>5.377999999999999</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9">
-        <v>2020</v>
-      </c>
-      <c r="B9">
-        <v>1995</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>6.628999999999999</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>1.32</v>
+        <v>1.150550010617966</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -13713,7 +13083,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.41</v>
+        <v>0.2692988929889298</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -13734,7 +13104,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1.213</v>
+        <v>1.024051444968231</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -13822,7 +13192,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1.604</v>
+        <v>1.354145521623284</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -13866,7 +13236,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0.6899999999999999</v>
+        <v>0.5825189588030334</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -14153,7 +13523,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0.1320000000000001</v>
+        <v>0.08670110701107013</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -14218,7 +13588,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1.371999999999999</v>
+        <v>1.158284074605451</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -14977,7 +14347,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.847</v>
+        <v>0.7825335342878673</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -15285,7 +14655,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.3700000000000001</v>
+        <v>0.3418387339864357</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -15329,7 +14699,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.1099999999999999</v>
+        <v>0.1016277317256969</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -15627,7 +14997,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.664</v>
+        <v>0.5658581081081081</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -15759,7 +15129,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.5199999999999999</v>
+        <v>0.4431418918918918</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -16235,7 +15605,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.423</v>
+        <v>0.133</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -16256,7 +15626,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.27</v>
+        <v>0.0009595735228787207</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -16300,7 +15670,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.612</v>
+        <v>0.0021750333185251</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -16344,7 +15714,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.369</v>
+        <v>0.004865393158596179</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -16855,16 +16225,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>2.87944</v>
+        <v>1.86</v>
       </c>
       <c r="E2">
-        <v>1.604</v>
+        <v>1.512402789886661</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.4944</v>
+        <v>1.18671431025597</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -16882,7 +16252,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1.6</v>
+        <v>1.027205882352941</v>
       </c>
       <c r="N2">
         <v>1.6818</v>
@@ -16990,7 +16360,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.4499999999999997</v>
+        <v>0.4243025283347861</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -17034,7 +16404,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.2400000000000002</v>
+        <v>0.2262946817785529</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -17058,7 +16428,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1.376</v>
+        <v>0.8833970588235293</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -17084,7 +16454,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.3540000000000001</v>
+        <v>0.2811140697474662</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -17102,7 +16472,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1.376</v>
+        <v>0.8833970588235296</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -17172,7 +16542,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.4799999999999998</v>
+        <v>0.381171619996564</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -17487,7 +16857,7 @@
         <v>0.9426000000000001</v>
       </c>
       <c r="E2">
-        <v>1.74</v>
+        <v>1.469497872340426</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -17514,7 +16884,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>6.409</v>
+        <v>3.765394905407419</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -17690,7 +17060,7 @@
         <v>10.3</v>
       </c>
       <c r="N6">
-        <v>0.1699999999999999</v>
+        <v>0.09987784894979886</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -17707,7 +17077,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1.785</v>
+        <v>1.507502127659574</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -17866,7 +17236,7 @@
         <v>3</v>
       </c>
       <c r="N10">
-        <v>0.1340000000000003</v>
+        <v>0.07872724564278286</v>
       </c>
     </row>
     <row r="11" spans="1:14">

</xml_diff>

<commit_message>
list of countries same as in other files
</commit_message>
<xml_diff>
--- a/grouped.xlsx
+++ b/grouped.xlsx
@@ -12,35 +12,36 @@
     <sheet name="BG" sheetId="3" r:id="rId3"/>
     <sheet name="CH" sheetId="4" r:id="rId4"/>
     <sheet name="CZ" sheetId="5" r:id="rId5"/>
-    <sheet name="DK" sheetId="6" r:id="rId6"/>
-    <sheet name="EE" sheetId="7" r:id="rId7"/>
-    <sheet name="FI" sheetId="8" r:id="rId8"/>
-    <sheet name="FR" sheetId="9" r:id="rId9"/>
-    <sheet name="DE" sheetId="10" r:id="rId10"/>
-    <sheet name="EL" sheetId="11" r:id="rId11"/>
-    <sheet name="IE" sheetId="12" r:id="rId12"/>
-    <sheet name="HU" sheetId="13" r:id="rId13"/>
-    <sheet name="IT" sheetId="14" r:id="rId14"/>
-    <sheet name="LV" sheetId="15" r:id="rId15"/>
-    <sheet name="LT" sheetId="16" r:id="rId16"/>
-    <sheet name="LU" sheetId="17" r:id="rId17"/>
-    <sheet name="NL" sheetId="18" r:id="rId18"/>
-    <sheet name="NO" sheetId="19" r:id="rId19"/>
-    <sheet name="PL" sheetId="20" r:id="rId20"/>
-    <sheet name="PT" sheetId="21" r:id="rId21"/>
-    <sheet name="RO" sheetId="22" r:id="rId22"/>
-    <sheet name="SK" sheetId="23" r:id="rId23"/>
-    <sheet name="SI" sheetId="24" r:id="rId24"/>
-    <sheet name="ES" sheetId="25" r:id="rId25"/>
-    <sheet name="SE" sheetId="26" r:id="rId26"/>
-    <sheet name="UK" sheetId="27" r:id="rId27"/>
+    <sheet name="DE" sheetId="6" r:id="rId6"/>
+    <sheet name="DK" sheetId="7" r:id="rId7"/>
+    <sheet name="EE" sheetId="8" r:id="rId8"/>
+    <sheet name="EL" sheetId="9" r:id="rId9"/>
+    <sheet name="ES" sheetId="10" r:id="rId10"/>
+    <sheet name="FI" sheetId="11" r:id="rId11"/>
+    <sheet name="FR" sheetId="12" r:id="rId12"/>
+    <sheet name="HR" sheetId="13" r:id="rId13"/>
+    <sheet name="HU" sheetId="14" r:id="rId14"/>
+    <sheet name="IE" sheetId="15" r:id="rId15"/>
+    <sheet name="IT" sheetId="16" r:id="rId16"/>
+    <sheet name="LT" sheetId="17" r:id="rId17"/>
+    <sheet name="LU" sheetId="18" r:id="rId18"/>
+    <sheet name="LV" sheetId="19" r:id="rId19"/>
+    <sheet name="NL" sheetId="20" r:id="rId20"/>
+    <sheet name="NO" sheetId="21" r:id="rId21"/>
+    <sheet name="PL" sheetId="22" r:id="rId22"/>
+    <sheet name="PT" sheetId="23" r:id="rId23"/>
+    <sheet name="RO" sheetId="24" r:id="rId24"/>
+    <sheet name="SE" sheetId="25" r:id="rId25"/>
+    <sheet name="SI" sheetId="26" r:id="rId26"/>
+    <sheet name="SK" sheetId="27" r:id="rId27"/>
+    <sheet name="UK" sheetId="28" r:id="rId28"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="14">
   <si>
     <t>year</t>
   </si>
@@ -1129,37 +1130,37 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="E2">
-        <v>1.091761329511611</v>
+        <v>0.03124145615252358</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.0472</v>
+        <v>0.9559728670694533</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.215</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0.4827</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1.45909117701958</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.4152</v>
+        <v>0.002825140233798355</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1176,34 +1177,34 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1.432770766307774</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.05859999999999976</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.02499999999999999</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>6.342954391395561</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.3265</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1220,13 +1221,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.181773636413628</v>
+        <v>0.2168089871057927</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.002900000000000125</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1235,19 +1236,19 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.09484880000000007</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1.444039301563543</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.2301</v>
+        <v>0.09486820905094874</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1261,37 +1262,37 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.052</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.8213695729362592</v>
+        <v>0.3585041075911092</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>3.684</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.257</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>1.9444</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>2.722507973110679</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>2.1849</v>
+        <v>0.1583879557826125</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1308,34 +1309,34 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1.733745432513732</v>
+        <v>1.113774708319268</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1.571700000000001</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.321</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0.90218</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.05597416185213721</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8709000000000002</v>
+        <v>0.02718138047443245</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1352,34 +1353,34 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>5.982442600266949</v>
+        <v>1.371567111022995</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.1583999999999994</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.1120000000000001</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>0.2334999999999998</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.3398901626416338</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>2.644740521910389</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>0.1594000000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1396,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>2.19727211839497</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1408,22 +1409,22 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0.07399999999999995</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0.1356099999999998</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.60781354575909</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>5.469259478089612</v>
+        <v>3.0404</v>
       </c>
       <c r="N8">
-        <v>0.04140000000000033</v>
+        <v>0.1658957659539316</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1437,37 +1438,37 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.03129999999999999</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1.20461255160326</v>
+        <v>0.02821808942808569</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.9992099999999988</v>
+        <v>0.06619672903549409</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.005100000000000104</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0.3774790000000006</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0.1498602350091676</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0.2143999999999995</v>
+        <v>0.04167611558646402</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1481,37 +1482,37 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.08640000000000003</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0.185182230583077</v>
+        <v>0.2194786199234713</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>4.118400000000002</v>
+        <v>0.05005459498621786</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.1108</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0.5912199999999999</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>5.327423169221067</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.05220000000000091</v>
+        <v>0.1119110440826019</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1525,37 +1526,37 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.6913933999999999</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2.094161836052704</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1.753159000000002</v>
+        <v>9.849880857691524</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.07519999999999971</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0.4382499999999983</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.9099046861617532</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.3640999999999996</v>
+        <v>0.02239100206549814</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1569,37 +1570,37 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.26985</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.03612267103894985</v>
+        <v>3.634575916324279</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>2.987100000000002</v>
+        <v>15.52674294193474</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.4000000000000001</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0.1565150000000006</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0.08918236207701816</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0.3110000000000008</v>
+        <v>0.1441633747054377</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1613,37 +1614,37 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.01509999999999989</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>5.590947090429791</v>
+        <v>0.1456691680797723</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2.482799999999997</v>
+        <v>3.563152009282573</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.15896</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0.4084500000000002</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1.618358834188772</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0.1632999999999987</v>
+        <v>0.05470001206427444</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1666,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1.567499999999999</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1675,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1.294461</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1687,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0.01250000000000018</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1758,16 +1759,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.86</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1.512402789886661</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.364722300140253</v>
+        <v>1.18671431025597</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1785,10 +1786,10 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1.027205882352941</v>
       </c>
       <c r="N2">
-        <v>0.501</v>
+        <v>1.6818</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1893,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.4243025283347861</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1937,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.2262946817785529</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1961,7 +1962,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>0.8833970588235293</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1987,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.2811140697474662</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -2002,10 +2003,10 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1.337767530306632</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>0.8833970588235296</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -2046,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.436332778702163</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -2075,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.381171619996564</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2090,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0.4083627287853578</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -2119,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.5878274894810657</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -2134,7 +2135,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.2733073449013549</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -2163,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.879163043478261</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -2178,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.230952697884478</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -2207,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.326908835904629</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2251,7 +2252,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.7433783309957919</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2266,7 +2267,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0.6752769194200144</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2387,16 +2388,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.137</v>
+        <v>0.9426000000000001</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1.469497872340426</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.178</v>
+        <v>3.509</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2408,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.0045</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -2417,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1.1896</v>
+        <v>3.765394905407419</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2484,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.427</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2505,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6519999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2572,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1.08</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2590,10 +2591,10 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>10.3</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.09987784894979886</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2610,13 +2611,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.507502127659574</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.1080000000000001</v>
+        <v>0.4130000000000003</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -2634,7 +2635,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>21.74</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -2678,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>17.67</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -2704,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.4629999999999999</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2722,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>6.549999999999997</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -2766,10 +2767,10 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>0.07872724564278286</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -2792,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1.253</v>
+        <v>0.7959999999999994</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -2810,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>2.990000000000002</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2836,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.055</v>
+        <v>1.762</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2880,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1.744</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2924,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.5850000000000009</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -3016,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.028</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3025,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.6536000000000001</v>
+        <v>0.3658</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3040,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.8195719120135363</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3060,7 +3061,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.106</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3084,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0.1874280879864636</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -3157,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.8409999999999996</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3201,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.8640000000000003</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3333,7 +3334,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.02729999999999944</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3377,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.4020000000000001</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -3421,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.306</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -3442,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -3465,7 +3466,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.0470000000000006</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -3509,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.427</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -3645,16 +3646,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.571</v>
+        <v>0.028</v>
       </c>
       <c r="E2">
-        <v>0.1421601409553641</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>10.27220785678001</v>
+        <v>0.6536000000000001</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3666,16 +3667,16 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.01938804780876494</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.8195719120135363</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>2.341590372388737</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3689,16 +3690,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.106</v>
       </c>
       <c r="E3">
-        <v>0.3131499608457322</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.6161164624478551</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -3713,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.1874280879864636</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.1461259185864089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3736,13 +3737,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1.284411902897416</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.8828547981158511</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3780,13 +3781,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.5895172278778387</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1.217505041331219</v>
+        <v>0.8409999999999996</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3807,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.3017869705226653</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3830,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.4712922740636997</v>
+        <v>0.8640000000000003</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3851,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.08390917347865584</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -3874,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.3272863014331223</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3886,7 +3887,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.09278565737051794</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -3930,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0.1038645418326693</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -3956,13 +3957,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>2.936650743931088</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.3043762603328047</v>
+        <v>0.02729999999999944</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3974,7 +3975,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.06162629482071715</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -4000,13 +4001,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.5169459671104155</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>3.107583432107509</v>
+        <v>0.4020000000000001</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -4018,7 +4019,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0.2437354581673307</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -4050,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>12.58334007435001</v>
+        <v>0.306</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -4062,7 +4063,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0.3102087649402391</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -4071,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.01358756502353242</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -4088,13 +4089,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1.834164056382145</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>9.820225474500873</v>
+        <v>0.0470000000000006</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -4106,7 +4107,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0.03739123505976084</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -4138,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2.920212024537041</v>
+        <v>0.427</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -4274,7 +4275,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.137</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -4283,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.178</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4304,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1.1896</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4392,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.6519999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -4459,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -4503,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.1080000000000001</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -4591,7 +4592,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.4629999999999999</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -4679,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1.253</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -4723,7 +4724,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.5839999999999999</v>
+        <v>1.055</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -4903,16 +4904,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.571</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.1421601409553641</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.716584362139918</v>
+        <v>10.27220785678001</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4924,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.01938804780876494</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -4933,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>2.341590372388737</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4950,13 +4951,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.3131499608457322</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.6161164624478551</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -4977,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.1461259185864089</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -4994,13 +4995,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1.284411902897416</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.8828547981158511</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -5038,13 +5039,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.5895172278778387</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1.217505041331219</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -5065,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>0.3017869705226653</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -5088,7 +5089,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.05341563786008224</v>
+        <v>0.4712922740636997</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -5109,7 +5110,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.08390917347865584</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -5132,7 +5133,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.3272863014331223</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -5144,7 +5145,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>0.09278565737051794</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -5188,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>0.1038645418326693</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -5214,13 +5215,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>2.936650743931088</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.3043762603328047</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -5232,7 +5233,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>0.06162629482071715</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -5258,13 +5259,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.5169459671104155</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>3.107583432107509</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -5276,7 +5277,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>0.2437354581673307</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -5308,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>12.58334007435001</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -5320,7 +5321,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>0.3102087649402391</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -5329,7 +5330,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>0.01358756502353242</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -5346,13 +5347,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1.834164056382145</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>9.820225474500873</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -5364,7 +5365,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>0.03739123505976084</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -5396,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2.920212024537041</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -5541,7 +5542,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.081</v>
+        <v>1.716584362139918</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -5717,7 +5718,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.05341563786008224</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -6164,13 +6165,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3.171819947400365</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2.486</v>
+        <v>0.081</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -6302,7 +6303,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.8689999999999998</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -6346,7 +6347,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.5739999999999998</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -6478,7 +6479,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1.763</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -6522,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>4.183</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -6566,7 +6567,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.8399999999999999</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -6610,7 +6611,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.848000000000001</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -6648,13 +6649,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1.490180052599636</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2.671999999999999</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -6799,7 +6800,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.642</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -7239,7 +7240,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.5839999999999999</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -8048,16 +8049,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.1116</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>2.1298</v>
+        <v>3.171819947400365</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.4112</v>
+        <v>2.486</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -8072,7 +8073,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.2074399596367306</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -8095,7 +8096,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1.4622</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8116,7 +8117,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1.280791120080726</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -8139,7 +8140,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1.1673</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -8160,7 +8161,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1.070768920282543</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -8183,13 +8184,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>6.664200000000001</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.07699999999999996</v>
+        <v>0.8689999999999998</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -8227,13 +8228,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>5.643000000000001</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.5739999999999998</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -8268,10 +8269,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.225</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.1429999999999971</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -8292,7 +8293,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>4.710006054490414</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -8359,13 +8360,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1.900600000000008</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1.763</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -8403,13 +8404,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.1890000000000001</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.1289000000000002</v>
+        <v>4.183</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -8447,13 +8448,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.3810000000000002</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.4179999999999999</v>
+        <v>0.8399999999999999</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -8488,7 +8489,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -8497,7 +8498,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1.848000000000001</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -8512,7 +8513,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0.4079939455095864</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -8532,16 +8533,16 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.205</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1.490180052599636</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2.671999999999999</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -8585,7 +8586,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.4849999999999999</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -8606,7 +8607,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0.359</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8686,7 +8687,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.826</v>
+        <v>0.642</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -8985,10 +8986,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.5760000000000001</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -9029,7 +9030,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.01899999999999999</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -9073,7 +9074,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.2329</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -9082,7 +9083,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1.176</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -9117,7 +9118,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.101</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -9126,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.8260000000000001</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -9138,7 +9139,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -9306,16 +9307,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.1116</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2.1298</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.897859531772575</v>
+        <v>1.4112</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -9330,10 +9331,10 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.4337548333226284</v>
+        <v>0.2074399596367306</v>
       </c>
       <c r="M2">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -9353,13 +9354,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1.4622</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.5276566332218507</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -9374,7 +9375,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1.280791120080726</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -9397,13 +9398,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1.1673</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.2709476031215161</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -9418,7 +9419,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1.070768920282543</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -9441,13 +9442,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.9999999999999999</v>
+        <v>6.664200000000001</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.2057681159420292</v>
+        <v>0.07699999999999996</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -9485,7 +9486,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5.643000000000001</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -9506,7 +9507,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>2.073764960284326</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -9526,10 +9527,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.225</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.1429999999999971</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -9550,7 +9551,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>4.710006054490414</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -9594,7 +9595,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.5634802063930462</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -9617,7 +9618,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1.900600000000008</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -9661,13 +9662,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.1890000000000001</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.1289000000000002</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -9705,13 +9706,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.3810000000000002</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.4179999999999999</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -9746,7 +9747,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -9755,7 +9756,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.1520624303232997</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -9770,7 +9771,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>0.4079939455095864</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -9790,7 +9791,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.205</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -9799,7 +9800,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.6117056856187292</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -9843,7 +9844,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.4849999999999999</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -9864,7 +9865,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>0.359</v>
       </c>
     </row>
   </sheetData>
@@ -9944,7 +9945,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.298</v>
+        <v>1.826</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -9959,7 +9960,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -10243,10 +10244,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.5760000000000001</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -10287,7 +10288,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.01899999999999999</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -10296,7 +10297,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.158</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -10314,7 +10315,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0.9399999999999999</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -10331,7 +10332,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.2329</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -10340,7 +10341,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1.176</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -10375,7 +10376,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.101</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -10384,7 +10385,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.4196</v>
+        <v>0.8260000000000001</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -10396,7 +10397,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -10573,13 +10574,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.897859531772575</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.053</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -10588,10 +10589,10 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.4337548333226284</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -10617,7 +10618,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.5276566332218507</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -10661,7 +10662,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.2709476031215161</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -10699,13 +10700,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.2057681159420292</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -10764,7 +10765,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>2.073764960284326</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -10808,7 +10809,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.04999999999999999</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -10852,7 +10853,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.5634802063930462</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -11013,7 +11014,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.1520624303232997</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -11057,7 +11058,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.6117056856187292</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -11072,7 +11073,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0.6000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -11193,16 +11194,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.02</v>
+        <v>0.405</v>
       </c>
       <c r="E2">
-        <v>0.03124145615252358</v>
+        <v>0.13</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.9559728670694533</v>
+        <v>0.708</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -11223,7 +11224,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.002825140233798355</v>
+        <v>1.569</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -11281,10 +11282,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.01999999999999996</v>
       </c>
       <c r="E4">
-        <v>0.2168089871057927</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -11311,7 +11312,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.09486820905094874</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -11328,7 +11329,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.3585041075911092</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -11355,7 +11356,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.1583879557826125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -11372,13 +11373,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1.113774708319268</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.639</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -11396,10 +11397,10 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1.862</v>
       </c>
       <c r="N6">
-        <v>0.02718138047443245</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -11416,7 +11417,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1.371567111022995</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -11440,7 +11441,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>5.686999999999999</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -11484,10 +11485,10 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>3.0404</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>0.1658957659539316</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -11504,13 +11505,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.02821808942808569</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.06619672903549409</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -11531,7 +11532,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0.04167611558646402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -11545,16 +11546,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.03870000000000001</v>
       </c>
       <c r="E10">
-        <v>0.2194786199234713</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.05005459498621786</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -11575,7 +11576,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.1119110440826019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -11592,13 +11593,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2.094161836052704</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>9.849880857691524</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -11619,7 +11620,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.02239100206549814</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -11636,13 +11637,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3.634575916324279</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>15.52674294193474</v>
+        <v>0.25</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -11663,7 +11664,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0.1441633747054377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -11680,13 +11681,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0.1456691680797723</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>3.563152009282573</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -11707,7 +11708,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0.05470001206427444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -11721,7 +11722,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -11822,22 +11823,22 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.405</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.708</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.053</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -11852,7 +11853,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1.569</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -11910,7 +11911,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.01999999999999996</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -11940,7 +11941,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -12007,7 +12008,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.639</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -12025,7 +12026,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1.862</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -12066,10 +12067,10 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>0.04999999999999999</v>
       </c>
       <c r="M7">
-        <v>5.686999999999999</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -12174,7 +12175,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.03870000000000001</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -12271,7 +12272,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -12330,7 +12331,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -12350,7 +12351,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -12451,6 +12452,635 @@
         <v>0</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0.298</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0.33</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>1965</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4">
+        <v>1970</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>2020</v>
+      </c>
+      <c r="B5">
+        <v>1975</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6">
+        <v>1980</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>2020</v>
+      </c>
+      <c r="B7">
+        <v>1985</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>2020</v>
+      </c>
+      <c r="B8">
+        <v>1990</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>2020</v>
+      </c>
+      <c r="B9">
+        <v>1995</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>2020</v>
+      </c>
+      <c r="B10">
+        <v>2000</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.158</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>2020</v>
+      </c>
+      <c r="B11">
+        <v>2005</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>2010</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0.4196</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>2020</v>
+      </c>
+      <c r="B13">
+        <v>2015</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>2020</v>
+      </c>
+      <c r="B14">
+        <v>2020</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2">
+        <v>1960</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>1.6837</v>
       </c>
       <c r="E2">
@@ -13718,7 +14348,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.3658</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -13739,7 +14369,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -13868,7 +14498,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>0.3780000000000001</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -13912,7 +14542,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -13956,7 +14586,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>1.245</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -14970,34 +15600,34 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1.091761329511611</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.2062</v>
+        <v>1.0472</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.215</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.4827</v>
       </c>
       <c r="K2">
-        <v>0.014</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1.45909117701958</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.5658581081081081</v>
+        <v>0.4152</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -15014,34 +15644,34 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1.432770766307774</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.05859999999999976</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.02499999999999999</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.109</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>6.342954391395561</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.3265</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -15058,13 +15688,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2.181773636413628</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.002900000000000125</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -15073,19 +15703,19 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.09484880000000007</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1.444039301563543</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.2301</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -15099,37 +15729,37 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.052</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.8213695729362592</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>3.684</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.257</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1.9444</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>2.722507973110679</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.4431418918918918</v>
+        <v>2.1849</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -15146,34 +15776,34 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.733745432513732</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1.571700000000001</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.321</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.90218</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>0.05597416185213721</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.8709000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -15190,34 +15820,34 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>5.982442600266949</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.08100000000000002</v>
+        <v>0.1583999999999994</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>0.1120000000000001</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.2334999999999998</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>0.3398901626416338</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>2.644740521910389</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>0.1594000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -15234,34 +15864,34 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0.265</v>
+        <v>2.19727211839497</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.07399999999999995</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.1356099999999998</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.60781354575909</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>5.469259478089612</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>0.04140000000000033</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -15275,37 +15905,37 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.03129999999999999</v>
       </c>
       <c r="E9">
-        <v>0.7869999999999999</v>
+        <v>1.20461255160326</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.9992099999999988</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.005100000000000104</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.3774790000000006</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>0.1498602350091676</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>0.2143999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -15319,37 +15949,37 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.08640000000000003</v>
       </c>
       <c r="E10">
-        <v>0.415</v>
+        <v>0.185182230583077</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.392</v>
+        <v>4.118400000000002</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.1108</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>0.5912199999999999</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>5.327423169221067</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>0.05220000000000091</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -15363,7 +15993,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.6913933999999999</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -15372,28 +16002,28 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1.753159000000002</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.07519999999999971</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>0.4382499999999983</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>0.9099046861617532</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>0.3640999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -15407,37 +16037,37 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.26985</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.03612267103894985</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>2.987100000000002</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.4000000000000001</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>0.1565150000000006</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>0.08918236207701816</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>0.3110000000000008</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -15451,37 +16081,37 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.01509999999999989</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>5.590947090429791</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2.482799999999997</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>0.15896</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.4084500000000002</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1.618358834188772</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>0.1632999999999987</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -15504,7 +16134,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1.567499999999999</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -15513,7 +16143,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1.294461</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -15525,7 +16155,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>0.01250000000000018</v>
       </c>
     </row>
   </sheetData>
@@ -15605,7 +16235,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.133</v>
+        <v>0.2062</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -15617,7 +16247,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.014</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -15626,7 +16256,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.0009595735228787207</v>
+        <v>0.5658581081081081</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -15670,7 +16300,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.0021750333185251</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -15714,7 +16344,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.004865393158596179</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -15758,7 +16388,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>0.4431418918918918</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -15825,7 +16455,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.08100000000000002</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -15863,13 +16493,13 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.265</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -15907,7 +16537,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.7869999999999999</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -15951,13 +16581,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.415</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.392</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -16225,16 +16855,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.86</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1.512402789886661</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.18671431025597</v>
+        <v>0.133</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -16252,10 +16882,10 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1.027205882352941</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1.6818</v>
+        <v>0.0009595735228787207</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -16299,7 +16929,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.0021750333185251</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -16343,7 +16973,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.004865393158596179</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -16360,7 +16990,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.4243025283347861</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -16404,7 +17034,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.2262946817785529</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -16428,7 +17058,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0.8833970588235293</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -16454,7 +17084,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.2811140697474662</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -16472,7 +17102,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0.8833970588235296</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -16542,7 +17172,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.381171619996564</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -16854,16 +17484,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.9426000000000001</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1.469497872340426</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>3.509</v>
+        <v>1.364722300140253</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -16875,7 +17505,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.0045</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -16884,7 +17514,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>3.765394905407419</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -16951,7 +17581,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.427</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -17057,10 +17687,10 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>10.3</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0.09987784894979886</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -17077,13 +17707,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1.507502127659574</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.4130000000000003</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -17098,10 +17728,10 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1.337767530306632</v>
       </c>
       <c r="M7">
-        <v>21.74</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -17142,10 +17772,10 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.436332778702163</v>
       </c>
       <c r="M8">
-        <v>17.67</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -17186,10 +17816,10 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>0.4083627287853578</v>
       </c>
       <c r="M9">
-        <v>6.549999999999997</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -17215,7 +17845,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.5878274894810657</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -17230,13 +17860,13 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>0.2733073449013549</v>
       </c>
       <c r="M10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>0.07872724564278286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -17259,7 +17889,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.7959999999999994</v>
+        <v>0.879163043478261</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -17274,10 +17904,10 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>0.230952697884478</v>
       </c>
       <c r="M11">
-        <v>2.990000000000002</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -17303,7 +17933,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1.762</v>
+        <v>1.326908835904629</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -17347,7 +17977,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>1.744</v>
+        <v>0.7433783309957919</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -17362,7 +17992,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>0.6752769194200144</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -17391,7 +18021,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.5850000000000009</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>

</xml_diff>